<commit_message>
Add Item as unique identifier for part requirement
</commit_message>
<xml_diff>
--- a/NewColNms.xlsx
+++ b/NewColNms.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
   <si>
     <t>MOQ</t>
   </si>
@@ -232,6 +232,78 @@
   </si>
   <si>
     <t>CIR.No...Sales.order.no.Production.order.no</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Rquired.Delivery.Date</t>
+  </si>
+  <si>
+    <t>KIT.Number</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>FG.Net.Req</t>
+  </si>
+  <si>
+    <t>SFG.Net.Req</t>
+  </si>
+  <si>
+    <t>Order.No</t>
+  </si>
+  <si>
+    <t>Order.Req</t>
+  </si>
+  <si>
+    <t>Req.Delivery.Date</t>
+  </si>
+  <si>
+    <t>KIT.Material</t>
+  </si>
+  <si>
+    <t>FG.Material</t>
+  </si>
+  <si>
+    <t>SFG.Material</t>
+  </si>
+  <si>
+    <t>Raw.Material</t>
+  </si>
+  <si>
+    <t>RM.Lead.Time</t>
+  </si>
+  <si>
+    <t>Material.Description</t>
+  </si>
+  <si>
+    <t>Storage.Location</t>
+  </si>
+  <si>
+    <t>Subcon.Stock</t>
+  </si>
+  <si>
+    <t>Min.Order.Qty</t>
+  </si>
+  <si>
+    <t>FG.SFG.Length</t>
+  </si>
+  <si>
+    <t>FG.SFG.Breadth</t>
+  </si>
+  <si>
+    <t>RM.Qty.Set</t>
+  </si>
+  <si>
+    <t>Open.PR.s</t>
+  </si>
+  <si>
+    <t>Open.PO.s</t>
   </si>
 </sst>
 </file>
@@ -273,9 +345,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,340 +664,496 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" customWidth="1"/>
+    <col min="13" max="13" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>47</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>46</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>44</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>42</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" t="s">
         <v>3</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>23</v>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M6" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N6" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P6" t="s">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q6" t="s">
         <v>27</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R6" t="s">
         <v>26</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S6" t="s">
         <v>25</v>
       </c>
-      <c r="P5" t="s">
+      <c r="T6" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="U6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K8" t="s">
         <v>17</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N8" t="s">
         <v>3</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O8" t="s">
         <v>15</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P8" t="s">
         <v>14</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H9" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K9" t="s">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M9" t="s">
         <v>4</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N9" t="s">
         <v>3</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O9" t="s">
         <v>2</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P9" t="s">
         <v>1</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q9" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>